<commit_message>
Running Random Forests Experiments
</commit_message>
<xml_diff>
--- a/Organized/Experiment_Runs_01-02_08_2020/ada/all_experiments.xlsx
+++ b/Organized/Experiment_Runs_01-02_08_2020/ada/all_experiments.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bachelor_Thesis\GitHub\BachelorThesis\Organized\experimentresults\ada\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bachelor_Thesis\GitHub\BachelorThesis\Organized\Experiment_Runs_01-02_08_2020\ada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2133FCC1-C0F5-462E-8DBF-255DF616237C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD93E413-E33F-4222-ABC4-14611207407A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27285" yWindow="1410" windowWidth="2400" windowHeight="585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,12 +94,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -127,16 +133,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -166,20 +187,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -194,7 +201,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7261B8CC-BF48-4304-A061-7A9D53102A68}" name="Table1" displayName="Table1" ref="A1:H2026" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7261B8CC-BF48-4304-A061-7A9D53102A68}" name="Table1" displayName="Table1" ref="A1:H2026" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:H2026" xr:uid="{C04DD25A-9BDD-406E-BBE5-B2DF24FBA756}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H2026">
     <sortCondition descending="1" ref="F1:F2026"/>
@@ -537,7 +544,7 @@
   <dimension ref="A1:H2026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,262 +586,262 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>50</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>0.94214876033057837</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>0.92982456140350878</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>0.9464285714285714</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>0.93805309734513276</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>0.94244505494505482</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>100</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>0.94214876033057837</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>0.92982456140350878</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>0.9464285714285714</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>0.93805309734513276</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>0.94244505494505482</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>75</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>0.93388429752066116</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>0.91379310344827602</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>0.9464285714285714</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>0.92982456140350878</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>0.93475274725274715</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>100</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>1.5</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>0.93388429752066116</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>0.9285714285714286</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>0.9285714285714286</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>0.9285714285714286</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>0.93351648351648364</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>50</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>1.5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>0.93388429752066116</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>0.96153846153846156</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>0.8928571428571429</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>0.92592592592592604</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>0.93104395604395596</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>50</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>0.7</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>0.92561983471074383</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>0.89830508474576276</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>0.9464285714285714</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>0.92173913043478262</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>0.9270604395604396</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>40</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>0.92561983471074383</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>0.91228070175438603</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>0.9285714285714286</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>0.92035398230088483</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>0.92582417582417598</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>100</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>0.8</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>0.92561983471074383</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>0.91228070175438603</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>0.9285714285714286</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>0.92035398230088483</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>0.92582417582417598</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>40</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>0.7</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>0.92561983471074383</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>0.91228070175438603</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>0.9285714285714286</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>0.92035398230088483</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>0.92582417582417598</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>40</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>0.6</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>0.91735537190082639</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>0.89655172413793083</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>0.9285714285714286</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>0.91228070175438603</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>0.91813186813186798</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>